<commit_message>
Fixed stadium arcadium file
</commit_message>
<xml_diff>
--- a/stadiumArcadium.xlsx
+++ b/stadiumArcadium.xlsx
@@ -1,22 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28908"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rowesis\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amol/Documents/Machine Learning Projects/TopicModelingSongLyrics/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14380" windowHeight="4420"/>
+    <workbookView xWindow="1420" yWindow="460" windowWidth="19000" windowHeight="13960"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -24,9 +30,48 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
-  <si>
-    <t xml:space="preserve">Getting born in the state of Mississippi
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="27">
+  <si>
+    <t xml:space="preserve">She's only eighteen
+Don't like the Rollin' Stones
+She took a short cut
+To bein' fully grown
+She got that mood ring
+Her little sister, Rose
+A smell of Springsteen
+A pair of pantyhose
+This talking picture show is leaking from a silhouette
+She said, "My man, you know, it's time to get your fingers wet"
+You hustle faster when you can't afford a cigarette
+The last I heard from you, why, you were screamin', "Handle it!"
+Knock the world
+Right off its feet and straight onto its head
+The book of love will long be laughing after you are dead
+Fascinated by the look of you and what was said
+Make a play for all the brightest minds in life will share
+I heard some P-Funk
+Out on the road again
+To get your head shrunk is what I recommend
+It's in your bloodline
+A perfect… </t>
+  </si>
+  <si>
+    <t>Album</t>
+  </si>
+  <si>
+    <t>Stadium Arcadium</t>
+  </si>
+  <si>
+    <t>Song</t>
+  </si>
+  <si>
+    <t>Dani California</t>
+  </si>
+  <si>
+    <t>Lyrics</t>
+  </si>
+  <si>
+    <t>"Getting born in the state of Mississippi
 Papa was a copper, and her mama was a hippy
 In Alabama she would swing a hammer
 Price you got to pay when you break the panorama
@@ -48,10 +93,13 @@
 She's a lover, baby, and a fighter
 Should've seen it coming when I got a little brighter
 With a name like Dani California
-Day was… </t>
-  </si>
-  <si>
-    <t xml:space="preserve">fCome to decide that the things that I tried
+Day was… "</t>
+  </si>
+  <si>
+    <t>Snow</t>
+  </si>
+  <si>
+    <t>"fCome to decide that the things that I tried
  Were in my life just to get high on
  When I sit alone come get a little known
  But I need more than myself this time
@@ -67,10 +115,10 @@
  All that I need to look inside
 Related
 Read more: Red Hot Chili Peppers - Snow (hey Oh) Lyrics | MetroLyrics 
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">All aboard, stitch in time
+"</t>
+  </si>
+  <si>
+    <t>"All aboard, stitch in time
 Get yours, got mine
 In a minute, I'll be there
 Sit tight, get square
@@ -102,10 +150,37 @@
 Pick it up and run like hell
 Little woman save me some
 Better get up on your run
-So much… </t>
-  </si>
-  <si>
-    <t xml:space="preserve">
+So much… "</t>
+  </si>
+  <si>
+    <t>Charlie</t>
+  </si>
+  <si>
+    <t>Hump De Bump</t>
+  </si>
+  <si>
+    <t>She's Only 18</t>
+  </si>
+  <si>
+    <t>Slow Cheetah</t>
+  </si>
+  <si>
+    <t>Torture Me</t>
+  </si>
+  <si>
+    <t>Strip My Mind</t>
+  </si>
+  <si>
+    <t>Especially in Michigan</t>
+  </si>
+  <si>
+    <t>Warlocks</t>
+  </si>
+  <si>
+    <t>C'mon Girl</t>
+  </si>
+  <si>
+    <t>"
 Bells around Saint Petersburg
 When I saw you
 I hope I get what you deserve
@@ -166,10 +241,10 @@
 Well I'm forming and I'm warning
 State of the art
 Until the clouds come crashing
-Stranger things have happened</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Forty detectives this week
+Stranger things have happened"</t>
+  </si>
+  <si>
+    <t>"Forty detectives this week
 Forty detectives strong
 Takin' a stroll down love street
 Strollin', is that so wrong?
@@ -200,34 +275,10 @@
 Hump de bump doop bodu
 Bump de hump doop bodu
 Hump de bump doop bop
-Bump de… </t>
-  </si>
-  <si>
-    <t xml:space="preserve">She's only eighteen
-Don't like the Rollin' Stones
-She took a short cut
-To bein' fully grown
-She got that mood ring
-Her little sister, Rose
-A smell of Springsteen
-A pair of pantyhose
-This talking picture show is leaking from a silhouette
-She said, "My man, you know, it's time to get your fingers wet"
-You hustle faster when you can't afford a cigarette
-The last I heard from you, why, you were screamin', "Handle it!"
-Knock the world
-Right off its feet and straight onto its head
-The book of love will long be laughing after you are dead
-Fascinated by the look of you and what was said
-Make a play for all the brightest minds in life will share
-I heard some P-Funk
-Out on the road again
-To get your head shrunk is what I recommend
-It's in your bloodline
-A perfect… </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Waking up dead inside of my head
+Bump de… "</t>
+  </si>
+  <si>
+    <t>"Waking up dead inside of my head
 Will never never do there is no med
 No medicine to take
 I've had a chance to be insane
@@ -260,10 +311,10 @@
 Looks like it's on today
 Slow cheetah come
 It's so euphoric
-No matter… </t>
-  </si>
-  <si>
-    <t>Because I'm happy to be sad
+No matter… "</t>
+  </si>
+  <si>
+    <t>"Because I'm happy to be sad
 I want it all I want it bad
 Oh oh
 It's what I know
@@ -291,10 +342,10 @@
 Is so
 All the leaves are turning brown
 The wind is pushing me around
-Let's go</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Oh, yeah yeah
+Let's go"</t>
+  </si>
+  <si>
+    <t>"Oh, yeah yeah
 Wow, wow, wow, wow, yeah
 Arthur J. did, indicate that
 The boulevard will never be 
@@ -320,10 +371,10 @@
 Won't you blow another compensator, hey
 (Ah, you only get what you bring)
 Oh yeah 
-Oh </t>
-  </si>
-  <si>
-    <t xml:space="preserve">
+Oh "</t>
+  </si>
+  <si>
+    <t>"
 Life is my friend 
 Rake it up to take it in 
 Wrap me in your cinnamon 
@@ -378,10 +429,10 @@
 Swimming with the mother duck 
 Deep in the mitten where 
 Lions and tigers come running 
-Just to steal your luck, yeah</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
+Just to steal your luck, yeah"</t>
+  </si>
+  <si>
+    <t>"
 Warlocks in wonderland 
 I've gotta megatropolis in my hand 
 And a, subterranean marching band 
@@ -439,10 +490,10 @@
 Coming up on it every day for 
 Look at me and it's what I stay for 
 A little locket of fantasy 
-That we believe in</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
+That we believe in"</t>
+  </si>
+  <si>
+    <t>"
 Everything inside of me
 Is burning up for you to see
 And if we should get into it
@@ -527,17 +578,33 @@
 Let's get it right (let's go)
 Let's get it right (let's go)
 Oh yeah she's with me and I'm your man
-If I can't find you no one can</t>
+If I can't find you no one can"</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -560,8 +627,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -569,7 +640,11 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="5">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -848,54 +923,158 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L1"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:12" ht="409.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="409" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="409" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="409" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="409" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="409" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="409" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>11</v>
+    </row>
+    <row r="8" spans="1:3" ht="409" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="409" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="409" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="409" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="409" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="409" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>